<commit_message>
Carga masiva de eventos desde Excel y asociación de usuario creador del evento
</commit_message>
<xml_diff>
--- a/docs/plantilla_eventos.xlsx
+++ b/docs/plantilla_eventos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhona\OneDrive\Escritorio\Programacion\Proyectos\event-management-api-dotnet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5800D1F-8503-48E3-8B10-521FF3FDF444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B046AF-3BF7-42DB-A625-800DDF8D114C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>title</t>
   </si>
@@ -62,26 +62,59 @@
     <t>longitude</t>
   </si>
   <si>
-    <t>Conferencia Dev</t>
-  </si>
-  <si>
-    <t>Tech Conference</t>
-  </si>
-  <si>
     <t>Auditorio Central</t>
   </si>
   <si>
-    <t>Calle 123 #45-67</t>
-  </si>
-  <si>
-    <t>Bogotá</t>
+    <t>Cartagena</t>
+  </si>
+  <si>
+    <t>Encuentro de fé</t>
+  </si>
+  <si>
+    <t>Fé</t>
+  </si>
+  <si>
+    <t>25/05/2025  23:00:00 a. m.</t>
+  </si>
+  <si>
+    <t>Pereira</t>
+  </si>
+  <si>
+    <t>Facatativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calle 14 # 1 - 3 </t>
+  </si>
+  <si>
+    <t>carrera 9 # 2 - 9</t>
+  </si>
+  <si>
+    <t>Edificio Grande</t>
+  </si>
+  <si>
+    <t>Colegio San Bartolomé</t>
+  </si>
+  <si>
+    <t>Dg. 8 # 8 - 3</t>
+  </si>
+  <si>
+    <t>Encuentro de auditores</t>
+  </si>
+  <si>
+    <t>Pescadores de Bolivar</t>
+  </si>
+  <si>
+    <t>Pesca</t>
+  </si>
+  <si>
+    <t>Auditores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +126,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -469,70 +508,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583070D7-D636-42C1-BCCB-445B0CAF9457}">
-  <dimension ref="B4:I6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="19.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="5" customWidth="1"/>
+    <col min="4" max="8" width="18.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4">
+        <v>852147</v>
+      </c>
+      <c r="H2" s="4">
+        <v>-7408175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45881.930555555555</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3">
-        <v>45833.375</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="G3" s="4">
+        <v>98729</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-7896541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4">
-        <v>460971</v>
-      </c>
-      <c r="I5" s="4">
-        <v>-7408175</v>
+      <c r="C4" s="3">
+        <v>45882.943055555559</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4">
+        <v>985632</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-3214569</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -543,6 +648,7 @@
       <c r="I6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementación de la geolocalización finalizada
</commit_message>
<xml_diff>
--- a/docs/plantilla_eventos.xlsx
+++ b/docs/plantilla_eventos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhona\OneDrive\Escritorio\Programacion\Proyectos\event-management-api-dotnet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B046AF-3BF7-42DB-A625-800DDF8D114C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4527874-51E9-4BDB-AFDC-34A41A9EC57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
+    <workbookView xWindow="-27060" yWindow="3210" windowWidth="21600" windowHeight="11295" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -62,52 +62,22 @@
     <t>longitude</t>
   </si>
   <si>
-    <t>Auditorio Central</t>
-  </si>
-  <si>
-    <t>Cartagena</t>
-  </si>
-  <si>
-    <t>Encuentro de fé</t>
-  </si>
-  <si>
-    <t>Fé</t>
-  </si>
-  <si>
     <t>25/05/2025  23:00:00 a. m.</t>
   </si>
   <si>
-    <t>Pereira</t>
-  </si>
-  <si>
-    <t>Facatativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calle 14 # 1 - 3 </t>
-  </si>
-  <si>
-    <t>carrera 9 # 2 - 9</t>
-  </si>
-  <si>
-    <t>Edificio Grande</t>
-  </si>
-  <si>
-    <t>Colegio San Bartolomé</t>
-  </si>
-  <si>
-    <t>Dg. 8 # 8 - 3</t>
-  </si>
-  <si>
-    <t>Encuentro de auditores</t>
-  </si>
-  <si>
-    <t>Pescadores de Bolivar</t>
-  </si>
-  <si>
-    <t>Pesca</t>
-  </si>
-  <si>
-    <t>Auditores</t>
+    <t>Papeleros</t>
+  </si>
+  <si>
+    <t>Encuentro de papeleros de Colombia</t>
+  </si>
+  <si>
+    <t>Central papelera</t>
+  </si>
+  <si>
+    <t>calle. 81 # 81 - 31</t>
+  </si>
+  <si>
+    <t>Bogotá</t>
   </si>
 </sst>
 </file>
@@ -168,11 +138,11 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,19 +478,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583070D7-D636-42C1-BCCB-445B0CAF9457}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="5" customWidth="1"/>
-    <col min="4" max="8" width="18.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="4" customWidth="1"/>
+    <col min="4" max="8" width="18.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -549,83 +519,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4">
-        <v>852147</v>
-      </c>
-      <c r="H2" s="4">
-        <v>-7408175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="3">
-        <v>45881.930555555555</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4">
-        <v>98729</v>
-      </c>
-      <c r="H3" s="4">
-        <v>-7896541</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>45882.943055555559</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4">
-        <v>985632</v>
-      </c>
-      <c r="H4" s="4">
-        <v>-3214569</v>
-      </c>
+      <c r="G2" s="1">
+        <v>4.6097099999999998</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-74.08175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -634,8 +572,8 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -643,9 +581,169 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Prueba final antes de Docker (CI/CD) con herramientas de devops
</commit_message>
<xml_diff>
--- a/docs/plantilla_eventos.xlsx
+++ b/docs/plantilla_eventos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhona\OneDrive\Escritorio\Programacion\Proyectos\event-management-api-dotnet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4527874-51E9-4BDB-AFDC-34A41A9EC57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0889B894-BCA2-4A35-BB61-CBAAEB887DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27060" yWindow="3210" windowWidth="21600" windowHeight="11295" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{900F8099-A353-4B59-B90F-BD9BD1F920ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>title</t>
   </si>
@@ -62,22 +62,34 @@
     <t>longitude</t>
   </si>
   <si>
-    <t>25/05/2025  23:00:00 a. m.</t>
-  </si>
-  <si>
-    <t>Papeleros</t>
-  </si>
-  <si>
-    <t>Encuentro de papeleros de Colombia</t>
-  </si>
-  <si>
-    <t>Central papelera</t>
-  </si>
-  <si>
-    <t>calle. 81 # 81 - 31</t>
-  </si>
-  <si>
     <t>Bogotá</t>
+  </si>
+  <si>
+    <t>Musica clasica</t>
+  </si>
+  <si>
+    <t>Concierto musica clásica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media torta </t>
+  </si>
+  <si>
+    <t>Av. 26 15 - 15</t>
+  </si>
+  <si>
+    <t>Musica Instrumental</t>
+  </si>
+  <si>
+    <t>Concierto musica Peruana</t>
+  </si>
+  <si>
+    <t>Centro de convenciones Lima</t>
+  </si>
+  <si>
+    <t>Dg. 140 15 - 40</t>
+  </si>
+  <si>
+    <t>Lima</t>
   </si>
 </sst>
 </file>
@@ -519,15 +531,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
+      <c r="C2" s="3">
+        <v>45902.5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -536,24 +548,40 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.7110000000000003</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-74.042100000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1">
-        <v>4.6097099999999998</v>
-      </c>
-      <c r="H2" s="1">
-        <v>-74.08175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45916.5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-12.1211</v>
+      </c>
+      <c r="H3" s="1">
+        <v>-77.029700000000005</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>

</xml_diff>